<commit_message>
Completed my first EDA -- developed a model
</commit_message>
<xml_diff>
--- a/CH-75 Table Transformation.xlsx
+++ b/CH-75 Table Transformation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0EB37E-C238-4159-971E-CCC75C996B3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62CF4F03-C2F2-4652-8B89-EE9F508F5F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19290" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18760" yWindow="1660" windowWidth="18380" windowHeight="15410" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$2:$E$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$E$16</definedName>
+    <definedName name="_nData">EDA!$B$3:$E$20</definedName>
     <definedName name="_nP">EDA!$D$3:$D$20</definedName>
     <definedName name="_nQ">EDA!$E$3:$E$20</definedName>
   </definedNames>
@@ -128,6 +129,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00;\-0.00;0.00;@"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -158,13 +162,13 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Mono"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -183,8 +187,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -259,21 +269,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -313,14 +314,16 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
+    <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -913,16 +916,16 @@
   <sheetData>
     <row r="1" spans="1:11" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="I1" s="15" t="s">
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="I1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="15"/>
+      <c r="J1" s="17"/>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
@@ -1291,10 +1294,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17F57EE2-99F8-4950-8221-2DF0ED78E1ED}">
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1304,26 +1307,26 @@
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="9.88671875" customWidth="1"/>
     <col min="5" max="5" width="10.77734375" customWidth="1"/>
-    <col min="6" max="6" width="12.77734375" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="20.88671875" customWidth="1"/>
     <col min="9" max="9" width="11.6640625" customWidth="1"/>
     <col min="10" max="10" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.44140625" customWidth="1"/>
+    <col min="11" max="12" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="I1" s="15" t="s">
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="I1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="15"/>
+      <c r="J1" s="17"/>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
@@ -1596,7 +1599,7 @@
       <c r="F16" s="10"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" s="7">
         <v>45422</v>
       </c>
@@ -1612,7 +1615,7 @@
       <c r="F17" s="10"/>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" s="7">
         <v>45422</v>
       </c>
@@ -1628,7 +1631,7 @@
       <c r="F18" s="10"/>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B19" s="7">
         <v>45431</v>
       </c>
@@ -1644,7 +1647,7 @@
       <c r="F19" s="10"/>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B20" s="7">
         <v>45431</v>
       </c>
@@ -1659,33 +1662,38 @@
       </c>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
       <c r="H21" s="3"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B24">
         <f>B20-B16</f>
         <v>10</v>
       </c>
       <c r="H24" s="3"/>
     </row>
-    <row r="27" spans="2:11" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B27" s="16" t="s">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="H26">
+        <f>COLUMNS(_xlfn.ANCHORARRAY(H29))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B27" s="15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="2:11" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
-        <v>2</v>
-      </c>
-      <c r="C29" s="17" cm="1">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B29" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="16" cm="1">
         <f t="array" ref="C29:F39">_xlfn._xlws.FILTER(B3:E20,_nP=B29)</f>
         <v>45380</v>
       </c>
@@ -1699,7 +1707,7 @@
         <v>12</v>
       </c>
       <c r="H29" t="str" cm="1">
-        <f t="array" ref="H29:K29">TRANSPOSE(_xlfn.UNIQUE(D29:D39))</f>
+        <f t="array" ref="H29:K29">TRANSPOSE(_xlfn.UNIQUE(_xlfn.CHOOSECOLS(_xlfn.ANCHORARRAY(C29),2)))</f>
         <v>O02</v>
       </c>
       <c r="I29" t="str">
@@ -1712,8 +1720,8 @@
         <v>O06</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C30" s="17">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C30" s="16">
         <v>45385</v>
       </c>
       <c r="D30" t="str">
@@ -1728,22 +1736,22 @@
       <c r="G30" t="s">
         <v>18</v>
       </c>
-      <c r="H30" s="17" cm="1">
+      <c r="H30" s="16" cm="1">
         <f t="array" ref="H30:K30">_xlfn.BYCOL(_xlfn.ANCHORARRAY(H29),_xlfn.LAMBDA(_xlpm.c,_xlfn.TAKE(_xlfn._xlws.FILTER(B3:E20,(_nP=$B$29)*(_nQ&gt;0)*(C3:C20=_xlpm.c)),,1)))</f>
         <v>45380</v>
       </c>
-      <c r="I30" s="17">
+      <c r="I30" s="16">
         <v>45401</v>
       </c>
-      <c r="J30" s="17">
+      <c r="J30" s="16">
         <v>45409</v>
       </c>
-      <c r="K30" s="17">
+      <c r="K30" s="16">
         <v>45409</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C31" s="17">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C31" s="16">
         <v>45392</v>
       </c>
       <c r="D31" t="str">
@@ -1772,8 +1780,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C32" s="17">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C32" s="16">
         <v>45401</v>
       </c>
       <c r="D32" t="str">
@@ -1785,9 +1793,29 @@
       <c r="F32">
         <v>20</v>
       </c>
-    </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C33" s="17">
+      <c r="H32" cm="1">
+        <f t="array" ref="H32">_xlfn.LET(_xlpm.z, _xlfn.CHOOSECOLS(_xlfn.DROP(_xlfn._xlws.FILTER(_nData,($C$3:$C$20=H$29)),1),{1,4}),_xlpm.d,_xlfn.TAKE(_xlpm.z,,1)-H$30,_xlpm.q,-_xlfn.TAKE(_xlpm.z,,-1),SUM(_xlpm.q*_xlpm.d))</f>
+        <v>88</v>
+      </c>
+      <c r="I32" cm="1">
+        <f t="array" ref="I32">_xlfn.LET(_xlpm.z, _xlfn.CHOOSECOLS(_xlfn.DROP(_xlfn._xlws.FILTER(_nData,($C$3:$C$20=I$29)),1),{1,4}),_xlpm.d,_xlfn.TAKE(_xlpm.z,,1)-I$30,_xlpm.q,-_xlfn.TAKE(_xlpm.z,,-1),SUM(_xlpm.q*_xlpm.d))</f>
+        <v>379</v>
+      </c>
+      <c r="J32" cm="1">
+        <f t="array" ref="J32">_xlfn.LET(_xlpm.z, _xlfn.CHOOSECOLS(_xlfn.DROP(_xlfn._xlws.FILTER(_nData,($C$3:$C$20=J$29)),1),{1,4}),_xlpm.d,_xlfn.TAKE(_xlpm.z,,1)-J$30,_xlpm.q,-_xlfn.TAKE(_xlpm.z,,-1),SUM(_xlpm.q*_xlpm.d))</f>
+        <v>6</v>
+      </c>
+      <c r="K32" cm="1">
+        <f t="array" ref="K32">_xlfn.LET(_xlpm.z, _xlfn.CHOOSECOLS(_xlfn.DROP(_xlfn._xlws.FILTER(_nData,($C$3:$C$20=K$29)),1),{1,4}),_xlpm.d,_xlfn.TAKE(_xlpm.z,,1)-K$30,_xlpm.q,-_xlfn.TAKE(_xlpm.z,,-1),SUM(_xlpm.q*_xlpm.d))</f>
+        <v>191</v>
+      </c>
+      <c r="L32" s="18" cm="1">
+        <f t="array" aca="1" ref="L32" ca="1">SUM(OFFSET(H32,0,0,1,$H$26)/SUM(_xlfn.ANCHORARRAY(H31)))</f>
+        <v>12.072727272727272</v>
+      </c>
+    </row>
+    <row r="33" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C33" s="16">
         <v>45409</v>
       </c>
       <c r="D33" t="str">
@@ -1800,8 +1828,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C34" s="17">
+    <row r="34" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C34" s="16">
         <v>45409</v>
       </c>
       <c r="D34" t="str">
@@ -1814,8 +1842,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C35" s="17">
+    <row r="35" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C35" s="16">
         <v>45410</v>
       </c>
       <c r="D35" t="str">
@@ -1828,8 +1856,8 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C36" s="17">
+    <row r="36" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C36" s="16">
         <v>45414</v>
       </c>
       <c r="D36" t="str">
@@ -1842,8 +1870,8 @@
         <v>-13</v>
       </c>
     </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C37" s="17">
+    <row r="37" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C37" s="16">
         <v>45417</v>
       </c>
       <c r="D37" t="str">
@@ -1856,8 +1884,8 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C38" s="17">
+    <row r="38" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C38" s="16">
         <v>45422</v>
       </c>
       <c r="D38" t="str">
@@ -1870,8 +1898,8 @@
         <v>-11</v>
       </c>
     </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C39" s="17">
+    <row r="39" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C39" s="16">
         <v>45431</v>
       </c>
       <c r="D39" t="str">
@@ -1882,6 +1910,66 @@
       </c>
       <c r="F39">
         <v>-7</v>
+      </c>
+    </row>
+    <row r="42" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="E42" t="str" cm="1">
+        <f t="array" ref="E42:F42">I2:J2</f>
+        <v>Product</v>
+      </c>
+      <c r="F42" t="str">
+        <v>AVG Delivery Time</v>
+      </c>
+    </row>
+    <row r="43" spans="3:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F43" s="18">
+        <f ca="1">L32</f>
+        <v>12.072727272727272</v>
+      </c>
+    </row>
+    <row r="44" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="E44" s="18" t="str" cm="1">
+        <f t="array" ref="E44:E46">_xlfn._xlws.SORT(_xlfn.UNIQUE(_nP))</f>
+        <v>A</v>
+      </c>
+      <c r="F44" s="18">
+        <f t="dataTable" ref="F44:F46" dt2D="0" dtr="0" r1="B29" ca="1"/>
+        <v>12.072727272727272</v>
+      </c>
+      <c r="H44" t="b" cm="1">
+        <f t="array" ref="H44:I46">E44:F46=I3:J5</f>
+        <v>1</v>
+      </c>
+      <c r="I44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="E45" s="18" t="str">
+        <v>B</v>
+      </c>
+      <c r="F45" s="18">
+        <v>4.1842105263157894</v>
+      </c>
+      <c r="H45" t="b">
+        <v>1</v>
+      </c>
+      <c r="I45" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="E46" s="18" t="str">
+        <v>C</v>
+      </c>
+      <c r="F46" s="18">
+        <v>1</v>
+      </c>
+      <c r="H46" t="b">
+        <v>1</v>
+      </c>
+      <c r="I46" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Starting on my own single function
</commit_message>
<xml_diff>
--- a/CH-75 Table Transformation.xlsx
+++ b/CH-75 Table Transformation.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62CF4F03-C2F2-4652-8B89-EE9F508F5F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5272003C-48B0-4B87-8F2A-C7DC8EE39692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18760" yWindow="1660" windowWidth="18380" windowHeight="15410" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18760" yWindow="1660" windowWidth="18380" windowHeight="15410" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
+    <sheet name="MySingleFunction" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$2:$E$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">MySingleFunction!$B$2:$E$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$E$16</definedName>
     <definedName name="_nData">EDA!$B$3:$E$20</definedName>
     <definedName name="_nP">EDA!$D$3:$D$20</definedName>
@@ -66,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="19">
   <si>
     <t>Result</t>
   </si>
@@ -316,11 +318,11 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
@@ -916,16 +918,16 @@
   <sheetData>
     <row r="1" spans="1:11" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="I1" s="17" t="s">
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="I1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="17"/>
+      <c r="J1" s="19"/>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
@@ -1296,8 +1298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17F57EE2-99F8-4950-8221-2DF0ED78E1ED}">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView topLeftCell="B17" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1317,16 +1319,16 @@
   <sheetData>
     <row r="1" spans="1:11" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="I1" s="17" t="s">
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="I1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="17"/>
+      <c r="J1" s="19"/>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
@@ -1690,7 +1692,7 @@
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B29" s="19" t="s">
+      <c r="B29" s="18" t="s">
         <v>2</v>
       </c>
       <c r="C29" s="16" cm="1">
@@ -1794,22 +1796,22 @@
         <v>20</v>
       </c>
       <c r="H32" cm="1">
-        <f t="array" ref="H32">_xlfn.LET(_xlpm.z, _xlfn.CHOOSECOLS(_xlfn.DROP(_xlfn._xlws.FILTER(_nData,($C$3:$C$20=H$29)),1),{1,4}),_xlpm.d,_xlfn.TAKE(_xlpm.z,,1)-H$30,_xlpm.q,-_xlfn.TAKE(_xlpm.z,,-1),SUM(_xlpm.q*_xlpm.d))</f>
+        <f t="array" ref="H32">IFERROR(_xlfn.LET(_xlpm.z, _xlfn.CHOOSECOLS(_xlfn.DROP(_xlfn._xlws.FILTER(_nData,($C$3:$C$20=H$29)),1),{1,4}),_xlpm.d,_xlfn.TAKE(_xlpm.z,,1)-H$30,_xlpm.q,-_xlfn.TAKE(_xlpm.z,,-1),SUM(_xlpm.q*_xlpm.d)),"")</f>
         <v>88</v>
       </c>
       <c r="I32" cm="1">
-        <f t="array" ref="I32">_xlfn.LET(_xlpm.z, _xlfn.CHOOSECOLS(_xlfn.DROP(_xlfn._xlws.FILTER(_nData,($C$3:$C$20=I$29)),1),{1,4}),_xlpm.d,_xlfn.TAKE(_xlpm.z,,1)-I$30,_xlpm.q,-_xlfn.TAKE(_xlpm.z,,-1),SUM(_xlpm.q*_xlpm.d))</f>
+        <f t="array" ref="I32">IFERROR(_xlfn.LET(_xlpm.z, _xlfn.CHOOSECOLS(_xlfn.DROP(_xlfn._xlws.FILTER(_nData,($C$3:$C$20=I$29)),1),{1,4}),_xlpm.d,_xlfn.TAKE(_xlpm.z,,1)-I$30,_xlpm.q,-_xlfn.TAKE(_xlpm.z,,-1),SUM(_xlpm.q*_xlpm.d)),"")</f>
         <v>379</v>
       </c>
       <c r="J32" cm="1">
-        <f t="array" ref="J32">_xlfn.LET(_xlpm.z, _xlfn.CHOOSECOLS(_xlfn.DROP(_xlfn._xlws.FILTER(_nData,($C$3:$C$20=J$29)),1),{1,4}),_xlpm.d,_xlfn.TAKE(_xlpm.z,,1)-J$30,_xlpm.q,-_xlfn.TAKE(_xlpm.z,,-1),SUM(_xlpm.q*_xlpm.d))</f>
+        <f t="array" ref="J32">IFERROR(_xlfn.LET(_xlpm.z, _xlfn.CHOOSECOLS(_xlfn.DROP(_xlfn._xlws.FILTER(_nData,($C$3:$C$20=J$29)),1),{1,4}),_xlpm.d,_xlfn.TAKE(_xlpm.z,,1)-J$30,_xlpm.q,-_xlfn.TAKE(_xlpm.z,,-1),SUM(_xlpm.q*_xlpm.d)),"")</f>
         <v>6</v>
       </c>
       <c r="K32" cm="1">
-        <f t="array" ref="K32">_xlfn.LET(_xlpm.z, _xlfn.CHOOSECOLS(_xlfn.DROP(_xlfn._xlws.FILTER(_nData,($C$3:$C$20=K$29)),1),{1,4}),_xlpm.d,_xlfn.TAKE(_xlpm.z,,1)-K$30,_xlpm.q,-_xlfn.TAKE(_xlpm.z,,-1),SUM(_xlpm.q*_xlpm.d))</f>
+        <f t="array" ref="K32">IFERROR(_xlfn.LET(_xlpm.z, _xlfn.CHOOSECOLS(_xlfn.DROP(_xlfn._xlws.FILTER(_nData,($C$3:$C$20=K$29)),1),{1,4}),_xlpm.d,_xlfn.TAKE(_xlpm.z,,1)-K$30,_xlpm.q,-_xlfn.TAKE(_xlpm.z,,-1),SUM(_xlpm.q*_xlpm.d)),"")</f>
         <v>191</v>
       </c>
-      <c r="L32" s="18" cm="1">
+      <c r="L32" s="17" cm="1">
         <f t="array" aca="1" ref="L32" ca="1">SUM(OFFSET(H32,0,0,1,$H$26)/SUM(_xlfn.ANCHORARRAY(H31)))</f>
         <v>12.072727272727272</v>
       </c>
@@ -1922,17 +1924,17 @@
       </c>
     </row>
     <row r="43" spans="3:9" hidden="1" x14ac:dyDescent="0.3">
-      <c r="F43" s="18">
+      <c r="F43" s="17">
         <f ca="1">L32</f>
         <v>12.072727272727272</v>
       </c>
     </row>
     <row r="44" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="E44" s="18" t="str" cm="1">
+      <c r="E44" s="17" t="str" cm="1">
         <f t="array" ref="E44:E46">_xlfn._xlws.SORT(_xlfn.UNIQUE(_nP))</f>
         <v>A</v>
       </c>
-      <c r="F44" s="18">
+      <c r="F44" s="17">
         <f t="dataTable" ref="F44:F46" dt2D="0" dtr="0" r1="B29" ca="1"/>
         <v>12.072727272727272</v>
       </c>
@@ -1945,10 +1947,10 @@
       </c>
     </row>
     <row r="45" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="E45" s="18" t="str">
+      <c r="E45" s="17" t="str">
         <v>B</v>
       </c>
-      <c r="F45" s="18">
+      <c r="F45" s="17">
         <v>4.1842105263157894</v>
       </c>
       <c r="H45" t="b">
@@ -1959,10 +1961,10 @@
       </c>
     </row>
     <row r="46" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="E46" s="18" t="str">
+      <c r="E46" s="17" t="str">
         <v>C</v>
       </c>
-      <c r="F46" s="18">
+      <c r="F46" s="17">
         <v>1</v>
       </c>
       <c r="H46" t="b">
@@ -1971,6 +1973,398 @@
       <c r="I46" t="b">
         <v>1</v>
       </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="I1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E00E94F-C054-40CB-82C3-0A580ABFC2F2}">
+  <dimension ref="A1:K24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3" style="4" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" customWidth="1"/>
+    <col min="5" max="5" width="10.77734375" customWidth="1"/>
+    <col min="6" max="6" width="12.77734375" customWidth="1"/>
+    <col min="7" max="7" width="6.21875" customWidth="1"/>
+    <col min="8" max="8" width="20.88671875" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" customWidth="1"/>
+    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="I1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="19"/>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4"/>
+      <c r="B2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="7">
+        <v>45348</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="8">
+        <v>20</v>
+      </c>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="I3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="11">
+        <v>12.072727272727272</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4"/>
+      <c r="B4" s="7">
+        <v>45351</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="8">
+        <v>-20</v>
+      </c>
+      <c r="F4" s="9"/>
+      <c r="G4"/>
+      <c r="I4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" s="11">
+        <v>4.1842105263157894</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4"/>
+      <c r="B5" s="7">
+        <v>45380</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="8">
+        <v>12</v>
+      </c>
+      <c r="F5" s="9"/>
+      <c r="G5"/>
+      <c r="I5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="7">
+        <v>45382</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="8">
+        <v>19</v>
+      </c>
+      <c r="F6" s="9"/>
+      <c r="G6"/>
+      <c r="I6"/>
+      <c r="J6"/>
+    </row>
+    <row r="7" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4"/>
+      <c r="B7" s="7">
+        <v>45383</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="8">
+        <v>-19</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7"/>
+      <c r="I7"/>
+      <c r="J7"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B8" s="7">
+        <v>45385</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="8">
+        <v>-8</v>
+      </c>
+      <c r="F8" s="10"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B9" s="7">
+        <v>45392</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="8">
+        <v>-4</v>
+      </c>
+      <c r="F9" s="10"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B10" s="7">
+        <v>45401</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="8">
+        <v>20</v>
+      </c>
+      <c r="F10" s="10"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B11" s="7">
+        <v>45409</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="8">
+        <v>6</v>
+      </c>
+      <c r="F11" s="10"/>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B12" s="7">
+        <v>45409</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="8">
+        <v>17</v>
+      </c>
+      <c r="F12" s="10"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B13" s="7">
+        <v>45410</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="8">
+        <v>-6</v>
+      </c>
+      <c r="F13" s="10"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B14" s="7">
+        <v>45414</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="8">
+        <v>-13</v>
+      </c>
+      <c r="F14" s="10"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B15" s="7">
+        <v>45417</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="8">
+        <v>-6</v>
+      </c>
+      <c r="F15" s="10"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B16" s="7">
+        <v>45421</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="8">
+        <v>18</v>
+      </c>
+      <c r="F16" s="10"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17" s="7">
+        <v>45422</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="8">
+        <v>-11</v>
+      </c>
+      <c r="F17" s="10"/>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" s="7">
+        <v>45422</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="8">
+        <v>-9</v>
+      </c>
+      <c r="F18" s="10"/>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" s="7">
+        <v>45431</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="8">
+        <v>-7</v>
+      </c>
+      <c r="F19" s="10"/>
+      <c r="H19" s="3"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" s="7">
+        <v>45431</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="8">
+        <v>-9</v>
+      </c>
+      <c r="H20" s="3"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H22" s="3"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H24" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Single function. Too complicated, but it works
</commit_message>
<xml_diff>
--- a/CH-75 Table Transformation.xlsx
+++ b/CH-75 Table Transformation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5272003C-48B0-4B87-8F2A-C7DC8EE39692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8501B040-738A-4F75-ADD6-83F31DC317E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18760" yWindow="1660" windowWidth="18380" windowHeight="15410" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <definedName name="_nData">EDA!$B$3:$E$20</definedName>
     <definedName name="_nP">EDA!$D$3:$D$20</definedName>
     <definedName name="_nQ">EDA!$E$3:$E$20</definedName>
+    <definedName name="fx">_xlfn.LAMBDA(_xlpm.tbl,_xlpm.pdt,_xlpm.od,     _xlfn.LET(         _xlpm.ff, _xlfn._xlws.FILTER(_xlpm.tbl, (_xlfn.CHOOSECOLS(_xlpm.tbl, 3) = _xlpm.pdt) * (_xlfn.CHOOSECOLS(_xlpm.tbl, 2) = _xlpm.od)),         _xlpm.fff, _xlfn.DROP(_xlpm.ff,1),         _xlpm.ref,INDEX(_xlpm.ff,1,1),_xlpm.qref, INDEX(_xlpm.ff,1,4),         _xlpm.days, _xlfn.TAKE(_xlpm.fff,,1)-_xlpm.ref,_xlpm.qnt,-_xlfn.TAKE(_xlpm.fff,,-1),         _xlfn.VSTACK(SUM(_xlpm.days*_xlpm.qnt),SUM(_xlpm.qnt))     ) )</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -68,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="20">
   <si>
     <t>Result</t>
   </si>
@@ -125,6 +126,9 @@
   </si>
   <si>
     <t>Delivery</t>
+  </si>
+  <si>
+    <t>One function</t>
   </si>
 </sst>
 </file>
@@ -893,6 +897,35 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="755" row="8">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{287868E0-E9A0-4CCB-ACFF-2DDA17B7CC89}">
+  <we:reference id="wa200003696" version="1.3.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="WA200003696" version="1.3.0.0" store="WA200003696" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties>
+    <we:property name="projectV0_1-56c6e055-265e-4713-816e-a646dbb708de" value="{&quot;kind&quot;:&quot;AFEJSONBlobNode&quot;,&quot;id&quot;:&quot;{859F3DFE-C547-4E3F-B643-D0AF48BAF911}&quot;}"/>
+  </we:properties>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K24"/>
@@ -1298,8 +1331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17F57EE2-99F8-4950-8221-2DF0ED78E1ED}">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView topLeftCell="B17" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView topLeftCell="B26" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29:F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1986,10 +2019,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E00E94F-C054-40CB-82C3-0A580ABFC2F2}">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2002,7 +2035,7 @@
     <col min="6" max="6" width="12.77734375" customWidth="1"/>
     <col min="7" max="7" width="6.21875" customWidth="1"/>
     <col min="8" max="8" width="20.88671875" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" customWidth="1"/>
+    <col min="9" max="9" width="18.44140625" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" customWidth="1"/>
   </cols>
@@ -2194,6 +2227,10 @@
         <v>20</v>
       </c>
       <c r="F10" s="10"/>
+      <c r="H10" s="1" cm="1">
+        <f t="array" ref="H10:H11">fx(B3:E20,"A","O02")</f>
+        <v>88</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11" s="7">
@@ -2209,7 +2246,9 @@
         <v>6</v>
       </c>
       <c r="F11" s="10"/>
-      <c r="H11" s="3"/>
+      <c r="H11" s="1">
+        <v>12</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B12" s="7">
@@ -2241,7 +2280,18 @@
         <v>-6</v>
       </c>
       <c r="F13" s="10"/>
-      <c r="H13" s="1"/>
+      <c r="H13" s="1" cm="1">
+        <f t="array" ref="H13:H14">_xlfn.LAMBDA(_xlpm.tbl,_xlpm.pdt,_xlpm.od,
+    _xlfn.LET(
+        _xlpm.ff, _xlfn._xlws.FILTER(_xlpm.tbl, (_xlfn.CHOOSECOLS(_xlpm.tbl, 3) = _xlpm.pdt) * (_xlfn.CHOOSECOLS(_xlpm.tbl, 2) = _xlpm.od)),
+        _xlpm.fff, _xlfn.DROP(_xlpm.ff,1),
+        _xlpm.ref,INDEX(_xlpm.ff,1,1),_xlpm.qref, INDEX(_xlpm.ff,1,4),
+        _xlpm.days, _xlfn.TAKE(_xlpm.fff,,1)-_xlpm.ref,_xlpm.qnt,-_xlfn.TAKE(_xlpm.fff,,-1),
+        _xlfn.VSTACK(SUM(_xlpm.days*_xlpm.qnt),SUM(_xlpm.qnt))
+    )
+)(B3:E20, "A", "O02")</f>
+        <v>88</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14" s="7">
@@ -2257,7 +2307,9 @@
         <v>-13</v>
       </c>
       <c r="F14" s="10"/>
-      <c r="H14" s="1"/>
+      <c r="H14" s="1">
+        <v>12</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B15" s="7">
@@ -2291,7 +2343,7 @@
       <c r="F16" s="10"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" s="7">
         <v>45422</v>
       </c>
@@ -2305,9 +2357,24 @@
         <v>-11</v>
       </c>
       <c r="F17" s="10"/>
-      <c r="H17" s="3"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H17" s="12" t="str" cm="1">
+        <f t="array" ref="H17:I20">_xlfn.LET(
+_xlpm.tb, B3:E20,
+_xlpm.p, _xlfn._xlws.SORT(_xlfn.UNIQUE(D3:D20)),
+_xlpm.fy, _xlfn.LAMBDA(_xlpm.pa,
+           _xlfn.LET(
+           _xlpm.oi,_xlfn.UNIQUE(_xlfn.CHOOSECOLS(_xlfn._xlws.FILTER(_xlpm.tb,D3:D20=_xlpm.pa),2)),
+           _xlpm.za,_xlfn.DROP(_xlfn.REDUCE("",_xlpm.oi,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.HSTACK(_xlpm.a,fx(_xlpm.tb,_xlpm.pa,_xlpm.v)))),,1),
+           SUM(_xlfn.TAKE(_xlpm.za,1))/SUM(_xlfn.TAKE(_xlpm.za,-1)))),
+_xlfn.VSTACK(I2:J2,_xlfn.HSTACK(_xlpm.p,_xlfn.DROP(_xlfn.REDUCE("",_xlpm.p, _xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,_xlpm.fy(_xlpm.v)))),1)))
+)</f>
+        <v>Product</v>
+      </c>
+      <c r="I17" s="13" t="str">
+        <v>AVG Delivery Time</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" s="7">
         <v>45422</v>
       </c>
@@ -2321,9 +2388,21 @@
         <v>-9</v>
       </c>
       <c r="F18" s="10"/>
-      <c r="H18" s="3"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H18" s="6" t="str">
+        <v>A</v>
+      </c>
+      <c r="I18" s="11">
+        <v>12.072727272727272</v>
+      </c>
+      <c r="K18" t="b" cm="1">
+        <f t="array" ref="K18:L20">I3:J5=H18:I20</f>
+        <v>1</v>
+      </c>
+      <c r="L18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B19" s="7">
         <v>45431</v>
       </c>
@@ -2337,9 +2416,20 @@
         <v>-7</v>
       </c>
       <c r="F19" s="10"/>
-      <c r="H19" s="3"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H19" s="6" t="str">
+        <v>B</v>
+      </c>
+      <c r="I19" s="11">
+        <v>4.1842105263157894</v>
+      </c>
+      <c r="K19" t="b">
+        <v>1</v>
+      </c>
+      <c r="L19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B20" s="7">
         <v>45431</v>
       </c>
@@ -2352,19 +2442,78 @@
       <c r="E20" s="8">
         <v>-9</v>
       </c>
-      <c r="H20" s="3"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H20" s="6" t="str">
+        <v>C</v>
+      </c>
+      <c r="I20" s="11">
+        <v>1</v>
+      </c>
+      <c r="K20" t="b">
+        <v>1</v>
+      </c>
+      <c r="L20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
       <c r="H21" s="3"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
       <c r="H24" s="3"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="G25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="H27" s="12" t="str" cm="1">
+        <f t="array" ref="H27:I30">_xlfn.LET(
+_xlpm.tb, B3:E20,
+_xlpm.p, _xlfn._xlws.SORT(_xlfn.UNIQUE(D3:D20)),
+_xlpm.fz,_xlfn.LAMBDA(_xlpm.tbl,_xlpm.pdt,_xlpm.od,_xlfn.LET(_xlpm.ff,_xlfn._xlws.FILTER(_xlpm.tbl,(_xlfn.CHOOSECOLS(_xlpm.tbl,3)=_xlpm.pdt)*(_xlfn.CHOOSECOLS(_xlpm.tbl,2)=_xlpm.od)),_xlpm.fff,_xlfn.DROP(_xlpm.ff,1),_xlpm.ref,INDEX(_xlpm.ff,1,1),_xlpm.qref,INDEX(_xlpm.ff,1,4),_xlpm.days,_xlfn.TAKE(_xlpm.fff,,1)-_xlpm.ref,_xlpm.qnt,-_xlfn.TAKE(_xlpm.fff,,-1),_xlfn.VSTACK(SUM(_xlpm.days*_xlpm.qnt),SUM(_xlpm.qnt)))),
+_xlpm.fy, _xlfn.LAMBDA(_xlpm.pa,
+           _xlfn.LET(
+           _xlpm.oi,_xlfn.UNIQUE(_xlfn.CHOOSECOLS(_xlfn._xlws.FILTER(_xlpm.tb,D3:D20=_xlpm.pa),2)),
+           _xlpm.za,_xlfn.DROP(_xlfn.REDUCE("",_xlpm.oi,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.HSTACK(_xlpm.a,_xlpm.fz(_xlpm.tb,_xlpm.pa,_xlpm.v)))),,1),
+           SUM(_xlfn.TAKE(_xlpm.za,1))/SUM(_xlfn.TAKE(_xlpm.za,-1)))),
+_xlfn.VSTACK(I2:J2,_xlfn.HSTACK(_xlpm.p,_xlfn.DROP(_xlfn.REDUCE("",_xlpm.p, _xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,_xlpm.fy(_xlpm.v)))),1)))
+)</f>
+        <v>Product</v>
+      </c>
+      <c r="I27" s="13" t="str">
+        <v>AVG Delivery Time</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="H28" s="6" t="str">
+        <v>A</v>
+      </c>
+      <c r="I28" s="11">
+        <v>12.072727272727272</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="H29" s="6" t="str">
+        <v>B</v>
+      </c>
+      <c r="I29" s="11">
+        <v>4.1842105263157894</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="H30" s="6" t="str">
+        <v>C</v>
+      </c>
+      <c r="I30" s="11">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2374,4 +2523,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<AFEJSONBlob xmlns="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0">ewAiAHMAYwBoAGUAbQBhACIAOgAiAGgAdAB0AHAAOgAvAC8AcwBjAGgAZQBtAGEAcwAuAGEAZAB2AGEAbgBjAGUAZABmAG8AcgBtAHUAbABhAGUAbgB2AGkAcgBvAG4AbQBlAG4AdAAuAG8AZgBmAGkAYwBlAGEAcABwAHMALgBsAGkAdgBlAC4AYwBvAG0ALwBhAGYAZQBwAHIAbwBqAGUAYwB0AHMALwAwAC4AMgAiACwAIgBmAGkAbABlAHMAIgA6AFsAewAiAHAAYQB0AGgAIgA6ACIALwBwAHIAbwBqAGUAYwB0AHMALwBXAG8AcgBrAGIAbwBvAGsAIgAsACIAdABlAHgAdAAiADoAIgAvAC8AIAAtAC0ALQAgAFcAbwByAGsAYgBvAG8AawAgAG0AbwBkAHUAbABlACAALQAtAC0AXABuAC8ALwAgAEEAIABmAGkAbABlACAAbwBmACAAbgBhAG0AZQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AcwAgAG8AZgAgAHQAaABlACAAZgBvAHIAbQA6AFwAbgAvAC8AIAAgACAAIABuAGEAbQBlACAAPQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AOwBcAG4AIgB9AF0ALAAiAHAAcgBvAGoAZQBjAHQATgBhAG0AZQBzACIAOgBbAF0ALAAiAGwAbwBjAGEAbABlACIAOgB7ACIAbABpAHMAdABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHIAbwB3AFMAZQBwAGEAcgBhAHQAbwByACIAOgAiADsAIgAsACIAYwBvAGwAdQBtAG4AUwBlAHAAYQByAGEAdABvAHIAIgA6ACIALAAiACwAIgB0AGgAbwB1AHMAYQBuAGQAcwBTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHQAaABvAHUAcwBhAG4AZABzAFAAbwBzAGkAdABpAG8AbgBzACIAOgBbADMAXQAsACIAZABlAGMAaQBtAGEAbABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAuACIALAAiAGQAYQB0AGUATwByAGQAZQByACIAOgAiAEQATQBZACIALAAiAGMAdQByAHIAZQBuAGMAeQBTAHkAbQBiAG8AbAAiADoAIgAkACIALAAiAGkAcwBDAHUAcgByAGUAbgBjAHkAUwB5AG0AYgBvAGwATABlAGEAZAAiADoAdAByAHUAZQAsACIAaQBzAEMAdQByAHIAZQBuAGMAeQBTAGUAcABCAHkAUwBwAGEAYwBlACIAOgBmAGEAbABzAGUALAAiAHIAbwB3AEwAZQB0AHQAZQByACIAOgAiAFIAIgAsACIAYwBvAGwAdQBtAG4ATABlAHQAdABlAHIAIgA6ACIAQwAiACwAIgByAGMATABlAGYAdABCAHIAYQBjAGsAZQB0ACIAOgAiAFsAIgAsACIAcgBjAFIAaQBnAGgAdABCAHIAYQBjAGsAZQB0ACIAOgAiAF0AIgAsACIAcwB0AGEAdABlAG0AZQBuAHQAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIAOwAiACwAIgBsAG8AYwBhAGwAZQBOAGEAbQBlACIAOgAiAGUAbgAtAHUAcwAiAH0AfQA=</AFEJSONBlob>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{859F3DFE-C547-4E3F-B643-D0AF48BAF911}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Formatted my single function
</commit_message>
<xml_diff>
--- a/CH-75 Table Transformation.xlsx
+++ b/CH-75 Table Transformation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8501B040-738A-4F75-ADD6-83F31DC317E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{736BCFAC-437A-4F5E-9DDA-31929BAAAFEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19290" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -128,7 +128,7 @@
     <t>Delivery</t>
   </si>
   <si>
-    <t>One function</t>
+    <t>One function, formatted</t>
   </si>
 </sst>
 </file>
@@ -917,6 +917,9 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
@@ -2022,7 +2025,7 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2475,15 +2478,20 @@
     <row r="27" spans="2:12" x14ac:dyDescent="0.3">
       <c r="H27" s="12" t="str" cm="1">
         <f t="array" ref="H27:I30">_xlfn.LET(
-_xlpm.tb, B3:E20,
-_xlpm.p, _xlfn._xlws.SORT(_xlfn.UNIQUE(D3:D20)),
-_xlpm.fz,_xlfn.LAMBDA(_xlpm.tbl,_xlpm.pdt,_xlpm.od,_xlfn.LET(_xlpm.ff,_xlfn._xlws.FILTER(_xlpm.tbl,(_xlfn.CHOOSECOLS(_xlpm.tbl,3)=_xlpm.pdt)*(_xlfn.CHOOSECOLS(_xlpm.tbl,2)=_xlpm.od)),_xlpm.fff,_xlfn.DROP(_xlpm.ff,1),_xlpm.ref,INDEX(_xlpm.ff,1,1),_xlpm.qref,INDEX(_xlpm.ff,1,4),_xlpm.days,_xlfn.TAKE(_xlpm.fff,,1)-_xlpm.ref,_xlpm.qnt,-_xlfn.TAKE(_xlpm.fff,,-1),_xlfn.VSTACK(SUM(_xlpm.days*_xlpm.qnt),SUM(_xlpm.qnt)))),
-_xlpm.fy, _xlfn.LAMBDA(_xlpm.pa,
-           _xlfn.LET(
-           _xlpm.oi,_xlfn.UNIQUE(_xlfn.CHOOSECOLS(_xlfn._xlws.FILTER(_xlpm.tb,D3:D20=_xlpm.pa),2)),
-           _xlpm.za,_xlfn.DROP(_xlfn.REDUCE("",_xlpm.oi,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.HSTACK(_xlpm.a,_xlpm.fz(_xlpm.tb,_xlpm.pa,_xlpm.v)))),,1),
-           SUM(_xlfn.TAKE(_xlpm.za,1))/SUM(_xlfn.TAKE(_xlpm.za,-1)))),
-_xlfn.VSTACK(I2:J2,_xlfn.HSTACK(_xlpm.p,_xlfn.DROP(_xlfn.REDUCE("",_xlpm.p, _xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,_xlpm.fy(_xlpm.v)))),1)))
+     _xlpm.tb, B3:E20,
+     _xlpm.p, _xlfn._xlws.SORT(_xlfn.UNIQUE(D3:D20)),
+     _xlpm.fz, _xlfn.LAMBDA(_xlpm.tbl,_xlpm.pdt,_xlpm.od,
+           _xlfn.LET(_xlpm.ff,_xlfn._xlws.FILTER(_xlpm.tbl,(_xlfn.CHOOSECOLS(_xlpm.tbl,3)=_xlpm.pdt)*(_xlfn.CHOOSECOLS(_xlpm.tbl,2)=_xlpm.od)),
+               _xlpm.fff,_xlfn.DROP(_xlpm.ff,1),_xlpm.ref,INDEX(_xlpm.ff,1,1),
+               _xlpm.qref,INDEX(_xlpm.ff,1,4),
+               _xlpm.days,_xlfn.TAKE(_xlpm.fff,,1)-_xlpm.ref,
+               _xlpm.qnt,-_xlfn.TAKE(_xlpm.fff,,-1),
+              _xlfn.VSTACK(SUM(_xlpm.days*_xlpm.qnt),SUM(_xlpm.qnt)))
+               ),
+     _xlpm.fy, _xlfn.LAMBDA(_xlpm.pa,_xlfn.LET(_xlpm.oi,_xlfn.UNIQUE(_xlfn.CHOOSECOLS(_xlfn._xlws.FILTER(_xlpm.tb,D3:D20=_xlpm.pa),2)),
+                       _xlpm.za,_xlfn.DROP(_xlfn.REDUCE("",_xlpm.oi,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.HSTACK(_xlpm.a,_xlpm.fz(_xlpm.tb,_xlpm.pa,_xlpm.v)))),,1),
+                       SUM(_xlfn.TAKE(_xlpm.za,1))/SUM(_xlfn.TAKE(_xlpm.za,-1)))),
+                _xlfn.VSTACK(I2:J2,_xlfn.HSTACK(_xlpm.p,_xlfn.DROP(_xlfn.REDUCE("",_xlpm.p, _xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,_xlpm.fy(_xlpm.v)))),1)))
 )</f>
         <v>Product</v>
       </c>

</xml_diff>

<commit_message>
Quick look at alternate solution
</commit_message>
<xml_diff>
--- a/CH-75 Table Transformation.xlsx
+++ b/CH-75 Table Transformation.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{736BCFAC-437A-4F5E-9DDA-31929BAAAFEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{983EDE54-A544-4329-960C-22E3FBCFC0AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19290" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
     <sheet name="MySingleFunction" sheetId="3" r:id="rId3"/>
+    <sheet name="Alt" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Alt!$B$2:$E$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$2:$E$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">MySingleFunction!$B$2:$E$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$E$16</definedName>
@@ -69,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="20">
   <si>
     <t>Result</t>
   </si>
@@ -899,7 +901,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="755" row="8">
+  <wetp:taskpane dockstate="right" visibility="0" width="1586" row="8">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -2024,7 +2026,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E00E94F-C054-40CB-82C3-0A580ABFC2F2}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+    <sheetView topLeftCell="C13" workbookViewId="0">
       <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
@@ -2533,6 +2535,457 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9767041E-5EFB-49D5-AF1D-89C82136F09F}">
+  <dimension ref="A1:K27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3" style="4" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" customWidth="1"/>
+    <col min="5" max="5" width="10.77734375" customWidth="1"/>
+    <col min="6" max="6" width="12.77734375" customWidth="1"/>
+    <col min="7" max="7" width="6.21875" customWidth="1"/>
+    <col min="8" max="8" width="20.88671875" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" customWidth="1"/>
+    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="I1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="19"/>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4"/>
+      <c r="B2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="7">
+        <v>45348</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="8">
+        <v>20</v>
+      </c>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="I3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="11">
+        <v>12.072727272727272</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4"/>
+      <c r="B4" s="7">
+        <v>45351</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="8">
+        <v>-20</v>
+      </c>
+      <c r="F4" s="9"/>
+      <c r="G4"/>
+      <c r="I4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" s="11">
+        <v>4.1842105263157894</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4"/>
+      <c r="B5" s="7">
+        <v>45380</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="8">
+        <v>12</v>
+      </c>
+      <c r="F5" s="9"/>
+      <c r="G5"/>
+      <c r="I5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="7">
+        <v>45382</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="8">
+        <v>19</v>
+      </c>
+      <c r="F6" s="9"/>
+      <c r="G6"/>
+      <c r="I6"/>
+      <c r="J6"/>
+    </row>
+    <row r="7" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4"/>
+      <c r="B7" s="7">
+        <v>45383</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="8">
+        <v>-19</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7"/>
+      <c r="I7"/>
+      <c r="J7"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B8" s="7">
+        <v>45385</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="8">
+        <v>-8</v>
+      </c>
+      <c r="F8" s="10"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B9" s="7">
+        <v>45392</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="8">
+        <v>-4</v>
+      </c>
+      <c r="F9" s="10"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B10" s="7">
+        <v>45401</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="8">
+        <v>20</v>
+      </c>
+      <c r="F10" s="10"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B11" s="7">
+        <v>45409</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="8">
+        <v>6</v>
+      </c>
+      <c r="F11" s="10"/>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B12" s="7">
+        <v>45409</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="8">
+        <v>17</v>
+      </c>
+      <c r="F12" s="10"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B13" s="7">
+        <v>45410</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="8">
+        <v>-6</v>
+      </c>
+      <c r="F13" s="10"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B14" s="7">
+        <v>45414</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="8">
+        <v>-13</v>
+      </c>
+      <c r="F14" s="10"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B15" s="7">
+        <v>45417</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="8">
+        <v>-6</v>
+      </c>
+      <c r="F15" s="10"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B16" s="7">
+        <v>45421</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="8">
+        <v>18</v>
+      </c>
+      <c r="F16" s="10"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17" s="7">
+        <v>45422</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="8">
+        <v>-11</v>
+      </c>
+      <c r="F17" s="10"/>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" s="7">
+        <v>45422</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="8">
+        <v>-9</v>
+      </c>
+      <c r="F18" s="10"/>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" s="7">
+        <v>45431</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="8">
+        <v>-7</v>
+      </c>
+      <c r="F19" s="10"/>
+      <c r="H19" s="3"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" s="7">
+        <v>45431</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="8">
+        <v>-9</v>
+      </c>
+      <c r="H20" s="3"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H22" s="3"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C24" s="12" t="str" cm="1">
+        <f t="array" ref="C24:D27">_xlfn.LET(
+    _xlpm.p, D3:D20,
+    _xlpm.u, _xlfn._xlws.SORT(_xlfn.UNIQUE(_xlpm.p)),
+    _xlfn.HSTACK(
+        _xlfn.VSTACK(D2, _xlpm.u),
+        _xlfn.REDUCE(
+            J2,
+            _xlpm.u,
+            _xlfn.LAMBDA(_xlpm.i,_xlpm.x,
+                _xlfn.LET(
+                    _xlpm.m, _xlfn._xlws.FILTER(B3:E20, _xlpm.p = _xlpm.x),
+                    _xlpm.F, _xlfn.LAMBDA(_xlpm.j, INDEX(_xlpm.m, , _xlpm.j)),
+                    _xlpm.q, _xlpm.F(4),
+                    _xlfn.VSTACK(
+                        _xlpm.i,
+                        SUM(
+                            _xlfn.MAP(
+                                _xlfn.UNIQUE(_xlpm.F(2)),
+                                _xlfn.LAMBDA(_xlpm.a,
+                                    _xlfn.LET(_xlpm.n, _xlfn._xlws.FILTER(_xlfn.HSTACK(_xlpm.F(1), _xlpm.q), _xlpm.F(2) = _xlpm.a), SUM((_xlfn.SINGLE(_xlpm.n) - _xlfn.DROP(_xlpm.n, 1, -1)) * _xlfn.DROP(_xlpm.n, 1, 1)))
+                                )
+                            )
+                        ) / SUM(_xlpm.q * (_xlpm.q &gt; 0))
+                    )
+                )
+            )
+        )
+    )
+)</f>
+        <v>Product</v>
+      </c>
+      <c r="D24" s="13" t="str">
+        <v>AVG Delivery Time</v>
+      </c>
+      <c r="H24" s="3"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C25" s="6" t="str">
+        <v>A</v>
+      </c>
+      <c r="D25" s="11">
+        <v>12.072727272727272</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C26" s="6" t="str">
+        <v>B</v>
+      </c>
+      <c r="D26" s="11">
+        <v>4.1842105263157894</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C27" s="6" t="str">
+        <v>C</v>
+      </c>
+      <c r="D27" s="11">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="I1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <AFEJSONBlob xmlns="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0">ewAiAHMAYwBoAGUAbQBhACIAOgAiAGgAdAB0AHAAOgAvAC8AcwBjAGgAZQBtAGEAcwAuAGEAZAB2AGEAbgBjAGUAZABmAG8AcgBtAHUAbABhAGUAbgB2AGkAcgBvAG4AbQBlAG4AdAAuAG8AZgBmAGkAYwBlAGEAcABwAHMALgBsAGkAdgBlAC4AYwBvAG0ALwBhAGYAZQBwAHIAbwBqAGUAYwB0AHMALwAwAC4AMgAiACwAIgBmAGkAbABlAHMAIgA6AFsAewAiAHAAYQB0AGgAIgA6ACIALwBwAHIAbwBqAGUAYwB0AHMALwBXAG8AcgBrAGIAbwBvAGsAIgAsACIAdABlAHgAdAAiADoAIgAvAC8AIAAtAC0ALQAgAFcAbwByAGsAYgBvAG8AawAgAG0AbwBkAHUAbABlACAALQAtAC0AXABuAC8ALwAgAEEAIABmAGkAbABlACAAbwBmACAAbgBhAG0AZQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AcwAgAG8AZgAgAHQAaABlACAAZgBvAHIAbQA6AFwAbgAvAC8AIAAgACAAIABuAGEAbQBlACAAPQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AOwBcAG4AIgB9AF0ALAAiAHAAcgBvAGoAZQBjAHQATgBhAG0AZQBzACIAOgBbAF0ALAAiAGwAbwBjAGEAbABlACIAOgB7ACIAbABpAHMAdABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHIAbwB3AFMAZQBwAGEAcgBhAHQAbwByACIAOgAiADsAIgAsACIAYwBvAGwAdQBtAG4AUwBlAHAAYQByAGEAdABvAHIAIgA6ACIALAAiACwAIgB0AGgAbwB1AHMAYQBuAGQAcwBTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHQAaABvAHUAcwBhAG4AZABzAFAAbwBzAGkAdABpAG8AbgBzACIAOgBbADMAXQAsACIAZABlAGMAaQBtAGEAbABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAuACIALAAiAGQAYQB0AGUATwByAGQAZQByACIAOgAiAEQATQBZACIALAAiAGMAdQByAHIAZQBuAGMAeQBTAHkAbQBiAG8AbAAiADoAIgAkACIALAAiAGkAcwBDAHUAcgByAGUAbgBjAHkAUwB5AG0AYgBvAGwATABlAGEAZAAiADoAdAByAHUAZQAsACIAaQBzAEMAdQByAHIAZQBuAGMAeQBTAGUAcABCAHkAUwBwAGEAYwBlACIAOgBmAGEAbABzAGUALAAiAHIAbwB3AEwAZQB0AHQAZQByACIAOgAiAFIAIgAsACIAYwBvAGwAdQBtAG4ATABlAHQAdABlAHIAIgA6ACIAQwAiACwAIgByAGMATABlAGYAdABCAHIAYQBjAGsAZQB0ACIAOgAiAFsAIgAsACIAcgBjAFIAaQBnAGgAdABCAHIAYQBjAGsAZQB0ACIAOgAiAF0AIgAsACIAcwB0AGEAdABlAG0AZQBuAHQAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIAOwAiACwAIgBsAG8AYwBhAGwAZQBOAGEAbQBlACIAOgAiAGUAbgAtAHUAcwAiAH0AfQA=</AFEJSONBlob>
 </file>

</xml_diff>